<commit_message>
Set ecmFolderPath to match object number
</commit_message>
<xml_diff>
--- a/acm/acm-config-server-repo/rules/drools-case-file-rules.xlsx
+++ b/acm/acm-config-server-repo/rules/drools-case-file-rules.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vladimir.cherepnalko\.arkcase\acm\acm-config-server-repo\rules\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82678D70-E0F4-43D5-AF1E-78A82FCBEA56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="111" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -85,7 +90,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">{
+      <t>{
     ExpressionParser ep = new SpelExpressionParser();
     Expression exp = ep.parseExpression(expression);
     EvaluationContext ec = new StandardEvaluationContext();
@@ -146,9 +151,6 @@
     <t>container?.folder?.cmisFolderId == null</t>
   </si>
   <si>
-    <t>setEcmFolderPath, '/Sites/acm/documentLibrary/Case Files/' + dateFormat('yyyyMMdd') + '_' + $caseFile.getId()</t>
-  </si>
-  <si>
     <t>Set Case Status</t>
   </si>
   <si>
@@ -174,37 +176,22 @@
   </si>
   <si>
     <t>setDueDate, addDays(180)</t>
+  </si>
+  <si>
+    <t>setEcmFolderPath, '/Sites/acm/documentLibrary/Case Files/'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -271,209 +258,221 @@
     </fill>
   </fills>
   <borders count="13">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="4" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="6" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="7" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="8" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="12" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -532,33 +531,341 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A2:D65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C14" activeCellId="0" pane="topLeft" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.1428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="100.423469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.719387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.70918367346939"/>
+    <col min="1" max="1" width="19.42578125"/>
+    <col min="2" max="2" width="24.28515625"/>
+    <col min="3" max="3" width="50.140625"/>
+    <col min="4" max="4" width="100.42578125"/>
+    <col min="5" max="5" width="66.7109375" customWidth="1"/>
+    <col min="6" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -568,7 +875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -578,7 +885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -588,7 +895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -598,7 +905,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -608,7 +915,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.7" outlineLevel="0" r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -618,7 +925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.7" outlineLevel="0" r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -628,7 +935,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -638,7 +945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -648,7 +955,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -658,7 +965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -668,7 +975,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -678,7 +985,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="247.75" outlineLevel="0" r="14">
+    <row r="14" spans="1:4" ht="330" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -688,7 +995,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8" t="s">
@@ -698,7 +1005,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
@@ -706,7 +1013,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="4" t="s">
@@ -716,7 +1023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="4" t="s">
@@ -724,7 +1031,7 @@
       </c>
       <c r="D19" s="10"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="11" t="s">
@@ -734,7 +1041,7 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="34.05" outlineLevel="0" r="21">
+    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>24</v>
       </c>
@@ -748,7 +1055,7 @@
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="22">
+    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>28</v>
@@ -760,7 +1067,7 @@
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>31</v>
@@ -769,147 +1076,121 @@
         <v>32</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="D24" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.7" outlineLevel="0" r="25">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="D25" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="26">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="D26" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="27">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="28">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="30">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="31">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="33">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.70918367346939"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.70918367346939"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>